<commit_message>
fixed evaluate for bayah
</commit_message>
<xml_diff>
--- a/docs/central_experiments.xlsx
+++ b/docs/central_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haida\Documents\GitHub\smartathon\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6672E8-C988-4EC8-B5A5-6EE5C0A7F59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21ACCA3D-2000-4D62-BFC4-72614CA38F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15930" yWindow="1845" windowWidth="20550" windowHeight="16905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11670" yWindow="3720" windowWidth="24810" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -51,17 +51,75 @@
     <t>batch size</t>
   </si>
   <si>
-    <t>meanAP</t>
+    <t>baseline- full finetune</t>
+  </si>
+  <si>
+    <t>resnet50</t>
+  </si>
+  <si>
+    <t>best validation meanAP</t>
+  </si>
+  <si>
+    <t>test meanAP</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>LinearLR</t>
+  </si>
+  <si>
+    <t>haidar</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>python src/train.py -m resnet50 -d "./data" -o "./test_model__unfz_lr005" --lr 0.005 -b 2</t>
+  </si>
+  <si>
+    <t>baseline- full finetune_increaseLR</t>
+  </si>
+  <si>
+    <t>babar</t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>python src/train.py -m resnet50 -d "./data" -o "./test_model_unfz_lr01" --lr 0.01 -b 2</t>
+  </si>
+  <si>
+    <t>0.12 at E5</t>
+  </si>
+  <si>
+    <t>baseline- full finetune_decreaseLR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,13 +142,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -369,52 +431,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="77.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>0.01</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>1E-3</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="0.12@Epoch5" xr:uid="{E3110AA9-DD8B-445A-8183-4183FD714B31}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>